<commit_message>
Started steel industry data collection and relationship setup
</commit_message>
<xml_diff>
--- a/excelData/globalData.xlsx
+++ b/excelData/globalData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A8A547EC-4C5D-4E43-B78E-0CB04DD97E15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="27640" windowHeight="16540"/>
+    <workbookView xWindow="675" yWindow="465" windowWidth="27645" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Processes" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="fuels" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Tanzer/GitHub/BlackBlox/globalData/fuels.tsv" thousands=" ">
+    <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/globalData/fuels.tsv" thousands=" ">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -39,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -128,21 +122,12 @@
     <t>HHV</t>
   </si>
   <si>
-    <t>biogenic</t>
-  </si>
-  <si>
     <t>meta-units</t>
   </si>
   <si>
-    <t>(mj/t)</t>
-  </si>
-  <si>
     <t>(t/t combusted)</t>
   </si>
   <si>
-    <t>(t/t)</t>
-  </si>
-  <si>
     <t>coal</t>
   </si>
   <si>
@@ -183,12 +168,27 @@
   </si>
   <si>
     <t>var meal mixer</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>steam</t>
+  </si>
+  <si>
+    <t>coke</t>
+  </si>
+  <si>
+    <t>(gj/t)</t>
+  </si>
+  <si>
+    <t>Eurofer electricity mix proxy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1020,7 +1020,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1030,13 +1030,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,19 +1050,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1073,22 +1073,22 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1099,22 +1099,22 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1125,22 +1125,22 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1213,21 +1213,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1238,54 +1238,57 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>34</v>
       </c>
       <c r="B3">
         <v>33.700000000000003</v>
       </c>
       <c r="C3">
-        <v>3.2</v>
+        <v>3.19</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>30</v>
       </c>
       <c r="C4">
-        <v>1.8</v>
+        <v>2.93</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -1297,9 +1300,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>45.3</v>
@@ -1311,9 +1314,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>21</v>
@@ -1322,6 +1325,48 @@
         <v>1.8</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>2.77</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>29.01</v>
+      </c>
+      <c r="C9">
+        <v>3.23</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.11</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
     </row>

</xml_diff>